<commit_message>
Adding THree Evalustion metrics for Tuning
</commit_message>
<xml_diff>
--- a/parameter_list/Agglomerative+parameterTuning.xlsx
+++ b/parameter_list/Agglomerative+parameterTuning.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,12 +446,17 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>calinski_harabasz_score</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>davies_bouldin_score</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>parameters_combinations</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>rank</t>
         </is>
       </c>
     </row>
@@ -462,33 +467,39 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7900151687435545</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>"3,euclidean,average"</t>
-        </is>
+        <v>0.2789490627547889</v>
+      </c>
+      <c r="C2" t="n">
+        <v>7821.728977223685</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>1.06287242850952</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>"3,euclidean,ward"</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>eval_datasets/test_2_eval.xlsx</t>
+          <t>eval_datasets/test_1_eval.xlsx</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7873551073615996</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>"3,manhattan,average"</t>
-        </is>
+        <v>0.4605969901439101</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2200.082270199993</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0.6030689835627047</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>"3,euclidean,complete"</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -498,15 +509,18 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.7524777728335076</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>"3,manhattan,complete"</t>
-        </is>
+        <v>0.7900151687435545</v>
+      </c>
+      <c r="C4" t="n">
+        <v>539.5168011753614</v>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>0.2998735945137385</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>"3,euclidean,average"</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -516,105 +530,123 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.7450514926598724</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>"3,manhattan,average"</t>
-        </is>
+        <v>0.7524777728335076</v>
+      </c>
+      <c r="C5" t="n">
+        <v>660.7881165843683</v>
       </c>
       <c r="D5" t="n">
-        <v>3</v>
+        <v>0.4057289160622577</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>"3,manhattan,complete"</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>eval_datasets/test_2_eval.xlsx</t>
+          <t>eval_datasets/test_1_eval.xlsx</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.7336845697308644</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>"3,euclidean,average"</t>
-        </is>
+        <v>0.7450514926598724</v>
+      </c>
+      <c r="C6" t="n">
+        <v>610.5149829166194</v>
       </c>
       <c r="D6" t="n">
-        <v>2</v>
+        <v>0.3823409017911434</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>"3,manhattan,average"</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>eval_datasets/test_3_eval.xlsx</t>
+          <t>eval_datasets/test_2_eval.xlsx</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.6790248925233603</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>"3,euclidean,average"</t>
-        </is>
+        <v>0.3297529116811677</v>
+      </c>
+      <c r="C7" t="n">
+        <v>6120.725641662055</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0.9671650765148169</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>"3,euclidean,ward"</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>eval_datasets/test_3_eval.xlsx</t>
+          <t>eval_datasets/test_2_eval.xlsx</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.6730601494851508</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>"3,manhattan,average"</t>
-        </is>
+        <v>0.5599471565244205</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1206.634924035146</v>
       </c>
       <c r="D8" t="n">
-        <v>2</v>
+        <v>0.5206835087392979</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>"3,euclidean,complete"</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>eval_datasets/test_4_eval.xlsx</t>
+          <t>eval_datasets/test_2_eval.xlsx</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.6637254014072674</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>"3,manhattan,average"</t>
-        </is>
+        <v>0.7336845697308644</v>
+      </c>
+      <c r="C9" t="n">
+        <v>535.536293877974</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>0.3691751804849007</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>"3,euclidean,average"</t>
+        </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>eval_datasets/test_4_eval.xlsx</t>
+          <t>eval_datasets/test_2_eval.xlsx</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.6090192210379256</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>"3,euclidean,average"</t>
-        </is>
+        <v>0.5649826201906503</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1188.901943034108</v>
       </c>
       <c r="D10" t="n">
-        <v>2</v>
+        <v>0.5611769956664775</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>"3,manhattan,complete"</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -624,51 +656,60 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.5649826201906503</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>"3,manhattan,complete"</t>
-        </is>
+        <v>0.7873551073615996</v>
+      </c>
+      <c r="C11" t="n">
+        <v>287.0972113100034</v>
       </c>
       <c r="D11" t="n">
-        <v>3</v>
+        <v>0.305926278826105</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>"3,manhattan,average"</t>
+        </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>eval_datasets/test_2_eval.xlsx</t>
+          <t>eval_datasets/test_3_eval.xlsx</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.5599471565244205</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>"3,euclidean,complete"</t>
-        </is>
+        <v>0.3385353445223021</v>
+      </c>
+      <c r="C12" t="n">
+        <v>8223.908197639621</v>
       </c>
       <c r="D12" t="n">
-        <v>4</v>
+        <v>0.8923090917525595</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>"3,euclidean,ward"</t>
+        </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>eval_datasets/test_4_eval.xlsx</t>
+          <t>eval_datasets/test_3_eval.xlsx</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.5493149780355437</v>
-      </c>
-      <c r="C13" t="inlineStr">
+        <v>0.3539922627492189</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1712.547115344986</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.6302781897366564</v>
+      </c>
+      <c r="E13" t="inlineStr">
         <is>
           <t>"3,euclidean,complete"</t>
         </is>
-      </c>
-      <c r="D13" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="14">
@@ -678,69 +719,81 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.4842450027645873</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>"3,manhattan,complete"</t>
-        </is>
+        <v>0.6790248925233603</v>
+      </c>
+      <c r="C14" t="n">
+        <v>199.5744768548442</v>
       </c>
       <c r="D14" t="n">
-        <v>3</v>
+        <v>0.3691286926736267</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>"3,euclidean,average"</t>
+        </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>eval_datasets/test_1_eval.xlsx</t>
+          <t>eval_datasets/test_3_eval.xlsx</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.4605969901439101</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>"3,euclidean,complete"</t>
-        </is>
+        <v>0.4842450027645873</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1323.673453672702</v>
       </c>
       <c r="D15" t="n">
-        <v>4</v>
+        <v>0.5203162854306486</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>"3,manhattan,complete"</t>
+        </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>eval_datasets/test_4_eval.xlsx</t>
+          <t>eval_datasets/test_3_eval.xlsx</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.362795979641472</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>"3,manhattan,complete"</t>
-        </is>
+        <v>0.6730601494851508</v>
+      </c>
+      <c r="C16" t="n">
+        <v>206.5566615213655</v>
       </c>
       <c r="D16" t="n">
-        <v>4</v>
+        <v>0.3994247883164554</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>"3,manhattan,average"</t>
+        </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>eval_datasets/test_3_eval.xlsx</t>
+          <t>eval_datasets/test_4_eval.xlsx</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.3539922627492189</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>"3,euclidean,complete"</t>
-        </is>
+        <v>0.353192212347119</v>
+      </c>
+      <c r="C17" t="n">
+        <v>6366.302243950843</v>
       </c>
       <c r="D17" t="n">
-        <v>4</v>
+        <v>0.8081520445489757</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>"3,euclidean,ward"</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -750,69 +803,81 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.353192212347119</v>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>"3,euclidean,ward"</t>
-        </is>
+        <v>0.5493149780355437</v>
+      </c>
+      <c r="C18" t="n">
+        <v>2540.581358420732</v>
       </c>
       <c r="D18" t="n">
-        <v>5</v>
+        <v>0.5246664979873296</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>"3,euclidean,complete"</t>
+        </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>eval_datasets/test_3_eval.xlsx</t>
+          <t>eval_datasets/test_4_eval.xlsx</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.3385353445223021</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>"3,euclidean,ward"</t>
-        </is>
+        <v>0.6090192210379256</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1680.006892396578</v>
       </c>
       <c r="D19" t="n">
-        <v>5</v>
+        <v>0.4463743192296767</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>"3,euclidean,average"</t>
+        </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>eval_datasets/test_2_eval.xlsx</t>
+          <t>eval_datasets/test_4_eval.xlsx</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.3297529116811677</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>"3,euclidean,ward"</t>
-        </is>
+        <v>0.362795979641472</v>
+      </c>
+      <c r="C20" t="n">
+        <v>5775.863201932922</v>
       </c>
       <c r="D20" t="n">
-        <v>5</v>
+        <v>0.757796438139723</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>"3,manhattan,complete"</t>
+        </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>eval_datasets/test_1_eval.xlsx</t>
+          <t>eval_datasets/test_4_eval.xlsx</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.2789490627547889</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>"3,euclidean,ward"</t>
-        </is>
+        <v>0.6637254014072674</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1972.434548032037</v>
       </c>
       <c r="D21" t="n">
-        <v>5</v>
+        <v>0.4632990372470223</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>"3,manhattan,average"</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>